<commit_message>
DD - Excel updated
</commit_message>
<xml_diff>
--- a/frontend/src/assets/legacy/Registration Excel.xlsx
+++ b/frontend/src/assets/legacy/Registration Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prama\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prama\projects\college\DarkDevil\frontend\src\assets\legacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7156A7A-A23C-4E3D-BA77-BEB0EDD8DDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D82DC5-583E-4E5C-A34C-5C95F3DBC6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34922,9 +34922,6 @@
     <t>MUSIC UNPLUGGED (Solo Instrumental)</t>
   </si>
   <si>
-    <t>DIVINE DISHES (Idea presentation)</t>
-  </si>
-  <si>
     <t>MARKETOMANIA</t>
   </si>
   <si>
@@ -34972,12 +34969,15 @@
   <si>
     <t>LYRICAL HUNT</t>
   </si>
+  <si>
+    <t xml:space="preserve">DIVINE DISHES </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -35049,6 +35049,13 @@
       <sz val="10"/>
       <color rgb="FF073763"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -35273,7 +35280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -35379,6 +35386,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -35608,8 +35616,8 @@
   </sheetPr>
   <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -35710,7 +35718,7 @@
       <c r="AO1" s="44"/>
       <c r="AP1" s="50"/>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" ht="13.2">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -35756,7 +35764,7 @@
       <c r="AO2" s="7"/>
       <c r="AP2" s="8"/>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" ht="16.2">
       <c r="A3" s="9"/>
       <c r="B3" s="51" t="s">
         <v>5</v>
@@ -35862,7 +35870,7 @@
         <v>0.92708333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" ht="15.6">
       <c r="A4" s="21"/>
       <c r="B4" s="22" t="s">
         <v>9</v>
@@ -35932,56 +35940,56 @@
         <v>30</v>
       </c>
       <c r="Y4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="Z4" s="24" t="s">
+      <c r="AA4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AA4" s="24" t="s">
+      <c r="AB4" s="24" t="s">
         <v>33</v>
-      </c>
-      <c r="AB4" s="24" t="s">
-        <v>34</v>
       </c>
       <c r="AC4" s="26"/>
       <c r="AD4" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE4" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="24" t="s">
+      <c r="AF4" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AF4" s="24" t="s">
+      <c r="AG4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AG4" s="24" t="s">
+      <c r="AH4" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AH4" s="24" t="s">
+      <c r="AI4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AI4" s="24" t="s">
+      <c r="AJ4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AJ4" s="24" t="s">
+      <c r="AK4" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AK4" s="24" t="s">
+      <c r="AL4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="AL4" s="24" t="s">
+      <c r="AM4" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AM4" s="24" t="s">
+      <c r="AN4" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AN4" s="27" t="s">
+      <c r="AO4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="AO4" s="24" t="s">
+      <c r="AP4" s="28" t="s">
         <v>46</v>
-      </c>
-      <c r="AP4" s="28" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:42" ht="13.2">
@@ -36040,7 +36048,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="53" t="s">
         <v>1</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -36135,7 +36143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" ht="13.2">
       <c r="A7" s="34"/>
       <c r="B7" s="35">
         <v>2</v>
@@ -36147,7 +36155,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="36" t="s">
+      <c r="K7" s="53" t="s">
         <v>1</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -36242,7 +36250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" ht="13.2">
       <c r="A8" s="34"/>
       <c r="B8" s="35">
         <v>3</v>
@@ -36349,7 +36357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" ht="13.2">
       <c r="A9" s="34"/>
       <c r="B9" s="35">
         <v>4</v>
@@ -36456,7 +36464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" ht="13.2">
       <c r="A10" s="34"/>
       <c r="B10" s="35">
         <v>5</v>
@@ -36563,7 +36571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" ht="13.2">
       <c r="A11" s="34"/>
       <c r="B11" s="35">
         <v>6</v>
@@ -36670,7 +36678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" ht="13.2">
       <c r="A12" s="34"/>
       <c r="B12" s="35">
         <v>7</v>
@@ -36777,7 +36785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" ht="13.2">
       <c r="A13" s="34"/>
       <c r="B13" s="35">
         <v>8</v>
@@ -36884,7 +36892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" ht="13.2">
       <c r="A14" s="34"/>
       <c r="B14" s="35">
         <v>9</v>
@@ -36991,7 +36999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" ht="13.2">
       <c r="A15" s="34"/>
       <c r="B15" s="35">
         <v>10</v>
@@ -37098,7 +37106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" ht="13.2">
       <c r="A16" s="34"/>
       <c r="B16" s="35">
         <v>11</v>
@@ -37205,7 +37213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:42" ht="13.2">
       <c r="A17" s="34"/>
       <c r="B17" s="35">
         <v>12</v>
@@ -37312,7 +37320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" ht="13.2">
       <c r="A18" s="34"/>
       <c r="B18" s="35">
         <v>13</v>
@@ -37419,7 +37427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" ht="13.2">
       <c r="A19" s="34"/>
       <c r="B19" s="35">
         <v>14</v>
@@ -37526,7 +37534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:42">
+    <row r="20" spans="1:42" ht="13.2">
       <c r="A20" s="34"/>
       <c r="B20" s="35">
         <v>15</v>
@@ -37633,7 +37641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:42">
+    <row r="21" spans="1:42" ht="13.2">
       <c r="A21" s="34"/>
       <c r="B21" s="35">
         <v>16</v>
@@ -37740,7 +37748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:42" ht="13.2">
       <c r="A22" s="34"/>
       <c r="B22" s="35">
         <v>17</v>
@@ -37847,7 +37855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:42" ht="13.2">
       <c r="A23" s="34"/>
       <c r="B23" s="35">
         <v>18</v>
@@ -37954,7 +37962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:42">
+    <row r="24" spans="1:42" ht="13.2">
       <c r="A24" s="34"/>
       <c r="B24" s="35">
         <v>20</v>
@@ -38061,7 +38069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:42" ht="13.2">
       <c r="A25" s="34"/>
       <c r="B25" s="35">
         <v>21</v>
@@ -38168,7 +38176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:42" ht="13.2">
       <c r="A26" s="34"/>
       <c r="B26" s="35">
         <v>22</v>
@@ -38275,7 +38283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:42">
+    <row r="27" spans="1:42" ht="13.2">
       <c r="A27" s="34"/>
       <c r="B27" s="35">
         <v>23</v>
@@ -38382,7 +38390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:42">
+    <row r="28" spans="1:42" ht="13.2">
       <c r="A28" s="34"/>
       <c r="B28" s="35">
         <v>24</v>

</xml_diff>